<commit_message>
✅ Updated employee mobile number in Emp_Details.xlsx
</commit_message>
<xml_diff>
--- a/Emp_Details.xlsx
+++ b/Emp_Details.xlsx
@@ -465,7 +465,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,7 +507,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="4">
-        <v>7483310758</v>
+        <v>7483310759</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update Excel data and code
</commit_message>
<xml_diff>
--- a/Emp_Details.xlsx
+++ b/Emp_Details.xlsx
@@ -465,7 +465,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,7 +507,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="4">
-        <v>7483310759</v>
+        <v>7483310758</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -518,7 +518,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="2">
-        <v>9876543202</v>
+        <v>9845594772</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update employee data and bot logic
</commit_message>
<xml_diff>
--- a/Emp_Details.xlsx
+++ b/Emp_Details.xlsx
@@ -119,7 +119,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -127,30 +127,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -462,156 +444,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>8117957331</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>7483310758</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>9845594772</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>6360581265</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>6360581288</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>6360184997</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>9876543206</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>9876543207</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>9876543208</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>9876543209</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Emp_Details.xlsx with new employee data
</commit_message>
<xml_diff>
--- a/Emp_Details.xlsx
+++ b/Emp_Details.xlsx
@@ -131,13 +131,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -447,7 +450,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -475,7 +478,7 @@
       <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>8117957331</v>
       </c>
     </row>
@@ -486,7 +489,7 @@
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>7483310758</v>
       </c>
     </row>

</xml_diff>